<commit_message>
New classes are added to read different type of Emails
</commit_message>
<xml_diff>
--- a/NASBAutomation/src/test/resources/CustomerPortalData.xlsx
+++ b/NASBAutomation/src/test/resources/CustomerPortalData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="3720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Email Domain:</t>
   </si>
   <si>
-    <t>gmail.com</t>
-  </si>
-  <si>
     <t>Defaults:</t>
   </si>
   <si>
@@ -250,13 +247,16 @@
     <t>2133577858</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Aksahhhhhh</t>
-  </si>
-  <si>
-    <t>AksahhhhhhQA</t>
+    <t>speridian.com</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>aditya</t>
+  </si>
+  <si>
+    <t>aditya1</t>
   </si>
 </sst>
 </file>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>12</v>
@@ -818,16 +818,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>17</v>
       </c>
       <c r="H7" s="12">
         <v>999909</v>
@@ -844,76 +844,76 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="G9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>26</v>
-      </c>
       <c r="J9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="25" t="s">
+      <c r="L9" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="M9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="25" t="s">
+      <c r="N9" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="O9" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="25" t="s">
-        <v>58</v>
-      </c>
       <c r="P9" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="19" t="str">
         <f>IF($C10="","",$C10&amp;$B$3&amp;$B$4&amp;$B10)</f>
-        <v>QARegUAT20220328R4g</v>
+        <v>QARegUAT20220328R4n</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="21" t="str">
         <f>IF($D10="","",$B$6 &amp; $D10 &amp; "@" &amp; $B$7)</f>
-        <v>adithya.bhaskar+QARegUAT20220328R4g@gmail.com</v>
+        <v>adithya.bhaskar+QARegUAT20220328R4n@speridian.com</v>
       </c>
       <c r="I10" s="22">
         <f>IF($D10="","",$B$5)</f>
@@ -923,22 +923,22 @@
         <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M10" t="s">
         <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -946,10 +946,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="19" t="str">
         <f t="shared" ref="D11:D18" si="0">IF($C11="","",$C11&amp;$B$3&amp;$B$4&amp;$B11)</f>
@@ -957,12 +957,12 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="21" t="str">
         <f t="shared" ref="H11:H18" si="1">IF($D11="","",$B$6 &amp; $D11 &amp; "@" &amp; $B$7)</f>
-        <v>adithya.bhaskar+MarshalUAT20220328R4unifi@gmail.com</v>
+        <v>adithya.bhaskar+MarshalUAT20220328R4unifi@speridian.com</v>
       </c>
       <c r="I11" s="22">
         <f t="shared" ref="I11:I18" si="2">IF($D11="","",$B$5)</f>
@@ -971,28 +971,28 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>35</v>
       </c>
       <c r="D12" s="19" t="str">
         <f t="shared" si="0"/>
         <v>QARegR14UAT20220328R4locreated</v>
       </c>
       <c r="E12" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+QARegR14UAT20220328R4locreated@gmail.com</v>
+        <v>adithya.bhaskar+QARegR14UAT20220328R4locreated@speridian.com</v>
       </c>
       <c r="I12" s="22">
         <f t="shared" si="2"/>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>39</v>
-      </c>
       <c r="C13" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="19" t="str">
         <f t="shared" si="0"/>
@@ -1015,12 +1015,12 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+MarshalUAT20220328R4primary@gmail.com</v>
+        <v>adithya.bhaskar+MarshalUAT20220328R4primary@speridian.com</v>
       </c>
       <c r="I13" s="22">
         <f t="shared" si="2"/>
@@ -1029,28 +1029,28 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>41</v>
-      </c>
       <c r="C14" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="19" t="str">
         <f t="shared" si="0"/>
         <v>QARegR14UAT20220328R4co</v>
       </c>
       <c r="E14" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>42</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>43</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+QARegR14UAT20220328R4co@gmail.com</v>
+        <v>adithya.bhaskar+QARegR14UAT20220328R4co@speridian.com</v>
       </c>
       <c r="I14" s="22">
         <f t="shared" si="2"/>
@@ -1062,10 +1062,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="19" t="str">
         <f t="shared" si="0"/>
@@ -1073,12 +1073,12 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+MaddyUAT20220328R4co2@gmail.com</v>
+        <v>adithya.bhaskar+MaddyUAT20220328R4co2@speridian.com</v>
       </c>
       <c r="I15" s="22">
         <f t="shared" si="2"/>
@@ -1090,27 +1090,27 @@
         <v>10</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="19" t="str">
         <f t="shared" si="0"/>
         <v>MarshalUAT20220328R4b</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H16" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+MarshalUAT20220328R4b@gmail.com</v>
+        <v>adithya.bhaskar+MarshalUAT20220328R4b@speridian.com</v>
       </c>
       <c r="I16" s="22">
         <f t="shared" si="2"/>
@@ -1122,27 +1122,27 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="19" t="str">
         <f t="shared" si="0"/>
         <v>MarshalUAT20220328R4co3</v>
       </c>
       <c r="E17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>50</v>
       </c>
       <c r="H17" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+MarshalUAT20220328R4co3@gmail.com</v>
+        <v>adithya.bhaskar+MarshalUAT20220328R4co3@speridian.com</v>
       </c>
       <c r="I17" s="22">
         <f t="shared" si="2"/>
@@ -1154,21 +1154,21 @@
         <v>15</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="19" t="str">
         <f t="shared" si="0"/>
         <v>MarshalUAT20220328R4c</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>adithya.bhaskar+MarshalUAT20220328R4c@gmail.com</v>
+        <v>adithya.bhaskar+MarshalUAT20220328R4c@speridian.com</v>
       </c>
       <c r="I18" s="22">
         <f t="shared" si="2"/>

</xml_diff>